<commit_message>
Update data set name in Plots.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F8E777-9860-477C-803A-6F9B770CF38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979B8A84-8708-4847-8F75-52AF5261620B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>Aciclovri observed</t>
   </si>
   <si>
-    <t>Aciclovir_Laskin 1982.Group A_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv</t>
-  </si>
-  <si>
     <t>Aciclovir</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>min</t>
+  </si>
+  <si>
+    <t>Aciclovir_Laskin 1982.Group A_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
   </si>
 </sst>
 </file>
@@ -560,21 +560,21 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -600,13 +600,13 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s">
         <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
@@ -615,7 +615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -633,16 +633,16 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -653,19 +653,19 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -698,19 +698,19 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -736,19 +736,19 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
       <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -759,12 +759,12 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -773,12 +773,12 @@
         <v>19</v>
       </c>
       <c r="L3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -813,9 +813,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -826,20 +826,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -855,22 +855,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -887,19 +887,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -918,34 +918,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -967,15 +967,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1178,6 +1169,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
@@ -1190,14 +1190,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1214,4 +1206,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Added (empty) sheet 'ObservedDataNames' to Plots.xlsx - Fix file path in writeDataNamesIntoExcel
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979B8A84-8708-4847-8F75-52AF5261620B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B916B818-2BBC-4706-985D-4CEDB4E3CE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="exportConfiguration" sheetId="11" r:id="rId4"/>
     <sheet name="dataTypes" sheetId="4" r:id="rId5"/>
     <sheet name="plotTypes" sheetId="10" r:id="rId6"/>
+    <sheet name="ObservedDataNames" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -559,7 +560,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -955,15 +956,25 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F50EB7-9B8D-43C6-8095-37A547673E3C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1170,21 +1181,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1209,9 +1219,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
proper handling of 'na'  in individual and administration protocol de… (#458)
* proper handling of 'na'  in individual and administration protocol definition

* - Added (empty) sheet 'ObservedDataNames' to Plots.xlsx
- Fix file path in writeDataNamesIntoExcel

* Add function loadObservedDataFromPKML

* Remove snapshot for R4.2
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979B8A84-8708-4847-8F75-52AF5261620B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B916B818-2BBC-4706-985D-4CEDB4E3CE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="exportConfiguration" sheetId="11" r:id="rId4"/>
     <sheet name="dataTypes" sheetId="4" r:id="rId5"/>
     <sheet name="plotTypes" sheetId="10" r:id="rId6"/>
+    <sheet name="ObservedDataNames" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -559,7 +560,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -955,15 +956,25 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F50EB7-9B8D-43C6-8095-37A547673E3C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1170,21 +1181,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1209,9 +1219,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Correctly apply values defined in column "aggregation"
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9325A80-8294-423C-99F7-D5199C62ACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4615E2D5-E288-4A65-A8E2-9049BE852345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>group</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>P1, P2, P3</t>
+  </si>
+  <si>
+    <t>aggregation</t>
   </si>
 </sst>
 </file>
@@ -564,18 +567,18 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -616,7 +619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -643,7 +646,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -666,7 +669,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -693,26 +696,27 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B8908D-615D-4618-BFCF-D7DBA10892F0}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.26171875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="9.26171875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -744,13 +748,16 @@
         <v>42</v>
       </c>
       <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -767,7 +774,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -777,11 +784,11 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -818,9 +825,9 @@
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -831,7 +838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -839,7 +846,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -860,14 +867,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -892,19 +899,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -923,34 +930,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -966,22 +973,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1184,6 +1182,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1196,14 +1203,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1222,6 +1221,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Change 'xAxisLimits' to 'xValuesLimit' as default for plotConfiguration of Plots.xlsx. (same for y axis)
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4615E2D5-E288-4A65-A8E2-9049BE852345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4EF48-10F7-4BEF-9FF1-982883EC001D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
@@ -166,12 +166,6 @@
     <t>Aciclovir PVB</t>
   </si>
   <si>
-    <t>xAxisLimits</t>
-  </si>
-  <si>
-    <t>yAxisLimits</t>
-  </si>
-  <si>
     <t>0, 24</t>
   </si>
   <si>
@@ -203,6 +197,12 @@
   </si>
   <si>
     <t>aggregation</t>
+  </si>
+  <si>
+    <t>xValuesLimits</t>
+  </si>
+  <si>
+    <t>yValuesLimits</t>
   </si>
 </sst>
 </file>
@@ -604,13 +604,13 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
         <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -657,7 +657,7 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -699,7 +699,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -742,19 +742,19 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" t="s">
-        <v>44</v>
-      </c>
       <c r="M1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -768,10 +768,10 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -785,7 +785,7 @@
         <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -843,7 +843,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -980,6 +980,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1182,15 +1191,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1203,6 +1203,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1221,14 +1229,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
X values limits (#513)
* Do not fail when a scenario cannot be simulated, but show a warning

Restructure of messages

* Fix NEWS.md

* Change 'xAxisLimits' to 'xValuesLimit' as default for plotConfiguration of Plots.xlsx. (same for y axis)
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4615E2D5-E288-4A65-A8E2-9049BE852345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4EF48-10F7-4BEF-9FF1-982883EC001D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
@@ -166,12 +166,6 @@
     <t>Aciclovir PVB</t>
   </si>
   <si>
-    <t>xAxisLimits</t>
-  </si>
-  <si>
-    <t>yAxisLimits</t>
-  </si>
-  <si>
     <t>0, 24</t>
   </si>
   <si>
@@ -203,6 +197,12 @@
   </si>
   <si>
     <t>aggregation</t>
+  </si>
+  <si>
+    <t>xValuesLimits</t>
+  </si>
+  <si>
+    <t>yValuesLimits</t>
   </si>
 </sst>
 </file>
@@ -604,13 +604,13 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
         <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -657,7 +657,7 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -699,7 +699,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -742,19 +742,19 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" t="s">
-        <v>44</v>
-      </c>
       <c r="M1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -768,10 +768,10 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -785,7 +785,7 @@
         <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -843,7 +843,7 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -980,6 +980,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1182,15 +1191,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1203,6 +1203,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1221,14 +1229,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Extend the vignette Update excel file
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4EF48-10F7-4BEF-9FF1-982883EC001D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A6A912-8C4D-48DA-BEE0-8B0CAF1F87F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>min</t>
   </si>
   <si>
-    <t>Aciclovir_Laskin 1982.Group A_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
-  </si>
-  <si>
     <t>P1, P2, P3</t>
   </si>
   <si>
@@ -203,6 +200,9 @@
   </si>
   <si>
     <t>yValuesLimits</t>
+  </si>
+  <si>
+    <t>Laskin 1982.Group A_Aciclovir_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
   </si>
 </sst>
 </file>
@@ -563,22 +563,22 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -619,7 +619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -646,7 +646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -657,7 +657,7 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
@@ -669,7 +669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -698,25 +698,25 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="9.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -742,13 +742,13 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" t="s">
-        <v>53</v>
-      </c>
       <c r="K1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" t="s">
         <v>42</v>
@@ -757,7 +757,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -774,7 +774,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -788,7 +788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -825,9 +825,9 @@
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -838,15 +838,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -867,14 +867,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -899,19 +899,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -930,34 +930,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -973,22 +973,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1191,6 +1182,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1203,14 +1203,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1229,6 +1221,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Drafted initial content for vignette on using Plots.xlsx (#505)
* Drafted initial content for vignette on using Plots.xlsx

* Save work in progress
+ add plotting workflow sketch
+ add paragraphs about excel based workflow

* Complete draft of plotting vignette

* Update remotes adress for PI

* Extend the vignette
Update excel file

* Rebuild articles

* Add to news

---------

Co-authored-by: Felix MIL <felix.mil@esqlabs.com>
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4EF48-10F7-4BEF-9FF1-982883EC001D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A6A912-8C4D-48DA-BEE0-8B0CAF1F87F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>min</t>
   </si>
   <si>
-    <t>Aciclovir_Laskin 1982.Group A_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
-  </si>
-  <si>
     <t>P1, P2, P3</t>
   </si>
   <si>
@@ -203,6 +200,9 @@
   </si>
   <si>
     <t>yValuesLimits</t>
+  </si>
+  <si>
+    <t>Laskin 1982.Group A_Aciclovir_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
   </si>
 </sst>
 </file>
@@ -563,22 +563,22 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -619,7 +619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -646,7 +646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -657,7 +657,7 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
@@ -669,7 +669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -698,25 +698,25 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="9.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -742,13 +742,13 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" t="s">
-        <v>53</v>
-      </c>
       <c r="K1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L1" t="s">
         <v>42</v>
@@ -757,7 +757,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -774,7 +774,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -788,7 +788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -825,9 +825,9 @@
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -838,15 +838,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -867,14 +867,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -899,19 +899,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -930,34 +930,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -973,22 +973,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1191,6 +1182,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1203,14 +1203,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1229,6 +1221,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Rename nSD to nsd (to match ospsuite's argument) + Update NEWS + pkgdown::build_site()
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600423AA-4B3A-404B-9B6B-94402D4AF3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B960C6-DEE3-4CBB-AB02-1CAE12D3BC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22665" yWindow="4515" windowWidth="13110" windowHeight="11595" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -202,9 +202,6 @@
     <t>Laskin 1982.Group A_Aciclovir_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
   </si>
   <si>
-    <t>nSD</t>
-  </si>
-  <si>
     <t>P4</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>AciclovirPop</t>
+  </si>
+  <si>
+    <t>nsd</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -689,7 +689,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -698,13 +698,13 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -727,7 +727,7 @@
         <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -762,8 +762,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +819,7 @@
         <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N1" t="s">
         <v>42</v>
@@ -869,10 +869,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -884,7 +884,7 @@
         <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M5">
         <v>1.96</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -947,10 +947,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1282,6 +1282,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
@@ -1290,15 +1299,6 @@
     <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1321,6 +1321,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1329,12 +1337,4 @@
     <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Small improvements to plotting vignette (#531)
* Small improvements to plotting vignette

* Add fig.showtext = TRUE on all vignettes so the images are rendered properly using showtext
+ reduce axis titles font size just a bit

* pkgdown::build_site()

---------

Co-authored-by: PavelBal <pavel.balazki@gmail.com>
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A6A912-8C4D-48DA-BEE0-8B0CAF1F87F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7544912D-421D-48BB-BDAB-F2ADA036B4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>group</t>
   </si>
@@ -151,9 +151,6 @@
     <t>P3</t>
   </si>
   <si>
-    <t>Aciclovr2</t>
-  </si>
-  <si>
     <t>plotGridName</t>
   </si>
   <si>
@@ -203,6 +200,12 @@
   </si>
   <si>
     <t>Laskin 1982.Group A_Aciclovir_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv_</t>
+  </si>
+  <si>
+    <t>Aciclovir2</t>
+  </si>
+  <si>
+    <t>Aciclovir.png</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -604,13 +607,13 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
         <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
@@ -637,13 +640,13 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -657,16 +660,16 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -742,19 +745,19 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" t="s">
-        <v>52</v>
-      </c>
       <c r="K1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
         <v>42</v>
-      </c>
-      <c r="M1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -768,10 +771,10 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -785,7 +788,7 @@
         <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -822,7 +825,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,12 +846,12 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -861,10 +864,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,13 +879,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1183,15 +1194,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
@@ -1200,6 +1202,15 @@
     <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1222,14 +1233,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1238,4 +1241,12 @@
     <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>